<commit_message>
update SP.xlsx and add report information
</commit_message>
<xml_diff>
--- a/template/SP.xlsx
+++ b/template/SP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E421C7B-3BF8-4371-8882-8577FC964B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E9C258-EA56-41C4-9943-27CA68982199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,8 +11,8 @@
     <sheet name="SP" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">SP!$A$1:$I$67</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">SP!$1:$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">SP!$A$1:$I$66</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">SP!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -159,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="[$-404]e&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,67 +175,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="18"/>
       <color theme="1"/>
-      <name val="微軟正黑體"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="標楷體"/>
+      <family val="4"/>
       <charset val="136"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="微軟正黑體"/>
-      <family val="2"/>
+      <name val="標楷體"/>
+      <family val="4"/>
       <charset val="136"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="微軟正黑體"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF31333F"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF31333F"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="微軟正黑體"/>
-      <family val="2"/>
+      <name val="標楷體"/>
+      <family val="4"/>
       <charset val="136"/>
     </font>
     <font>
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF31333F"/>
+      <name val="標楷體"/>
+      <family val="4"/>
       <charset val="136"/>
     </font>
   </fonts>
@@ -382,56 +361,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -462,7 +438,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>683748</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>91110</xdr:rowOff>
+      <xdr:rowOff>140806</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -512,7 +488,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>16599</xdr:rowOff>
+      <xdr:rowOff>41446</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -556,7 +532,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>335017</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>144100</xdr:rowOff>
+      <xdr:rowOff>160666</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -600,7 +576,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>41413</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>109905</xdr:rowOff>
+      <xdr:rowOff>134752</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -643,7 +619,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>94942</xdr:rowOff>
+      <xdr:rowOff>136356</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -679,15 +655,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>505239</xdr:colOff>
+      <xdr:colOff>521805</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>165653</xdr:rowOff>
+      <xdr:rowOff>190501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>62347</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>588066</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>52131</xdr:rowOff>
+      <xdr:rowOff>56924</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -710,8 +686,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1797326" y="12274827"/>
-          <a:ext cx="1495238" cy="400000"/>
+          <a:off x="1813892" y="10618305"/>
+          <a:ext cx="1358348" cy="363380"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -731,7 +707,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>489231</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>124241</xdr:rowOff>
+      <xdr:rowOff>149088</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -774,7 +750,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>488674</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>83267</xdr:rowOff>
+      <xdr:rowOff>116397</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1097,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A57" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1085,7 @@
     <col min="9" max="9" width="14.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.4">
       <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
@@ -1122,7 +1098,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
@@ -1135,29 +1111,16 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="21">
@@ -1166,7 +1129,7 @@
       </c>
       <c r="I4" s="21"/>
     </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
@@ -1179,7 +1142,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1192,8 +1155,8 @@
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="7"/>
@@ -1205,8 +1168,8 @@
       <c r="H7" s="7"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="7"/>
@@ -1218,8 +1181,8 @@
       <c r="H8" s="7"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
+    <row r="9" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1229,8 +1192,8 @@
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="7"/>
@@ -1242,8 +1205,8 @@
       <c r="H10" s="7"/>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
+    <row r="11" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1253,12 +1216,12 @@
       <c r="H11" s="7"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="9"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="7" t="s">
         <v>9</v>
       </c>
@@ -1268,12 +1231,12 @@
       <c r="H12" s="7"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="9"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="7" t="s">
         <v>10</v>
       </c>
@@ -1283,12 +1246,12 @@
       <c r="H13" s="7"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="9"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -1296,8 +1259,8 @@
       <c r="H14" s="7"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
+    <row r="15" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1307,14 +1270,14 @@
       <c r="H15" s="7"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
+    <row r="16" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="7"/>
       <c r="G16" s="25" t="s">
         <v>32</v>
@@ -1322,8 +1285,8 @@
       <c r="H16" s="25"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
+    <row r="17" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1333,8 +1296,8 @@
       <c r="H17" s="7"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
+    <row r="18" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1344,21 +1307,21 @@
       <c r="H18" s="7"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
+    <row r="19" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="9"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
+    <row r="20" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1368,8 +1331,8 @@
       <c r="H20" s="7"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="7"/>
@@ -1394,8 +1357,8 @@
       <c r="H22" s="23"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
+    <row r="23" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1405,8 +1368,8 @@
       <c r="H23" s="7"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
+    <row r="24" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1416,8 +1379,8 @@
       <c r="H24" s="7"/>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
+    <row r="25" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1427,8 +1390,8 @@
       <c r="H25" s="7"/>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
+    <row r="26" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1438,8 +1401,8 @@
       <c r="H26" s="7"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
+    <row r="27" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1449,8 +1412,8 @@
       <c r="H27" s="7"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
+    <row r="28" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1460,8 +1423,8 @@
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
+    <row r="29" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1471,8 +1434,8 @@
       <c r="H29" s="7"/>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
+    <row r="30" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1482,8 +1445,8 @@
       <c r="H30" s="7"/>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
+    <row r="31" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1493,8 +1456,8 @@
       <c r="H31" s="7"/>
       <c r="I31" s="8"/>
     </row>
-    <row r="32" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A32" s="6"/>
+    <row r="32" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1504,18 +1467,18 @@
       <c r="H32" s="7"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="15"/>
-    </row>
-    <row r="34" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
@@ -1528,396 +1491,372 @@
       <c r="H34" s="4"/>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A35" s="6"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
+    <row r="35" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
       <c r="I35" s="8"/>
     </row>
-    <row r="36" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A36" s="12" t="s">
+    <row r="36" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
       <c r="I36" s="8"/>
     </row>
-    <row r="37" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A37" s="6"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
+    <row r="37" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
       <c r="I37" s="8"/>
     </row>
-    <row r="38" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
+    <row r="39" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A40" s="12" t="s">
+    <row r="40" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="6"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
+    <row r="41" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A43" s="10" t="s">
+    <row r="43" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A45" s="6"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
+    <row r="45" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="9"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A46" s="6"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
+    <row r="46" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A46" s="9"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A47" s="6"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
+    <row r="47" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="9"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
       <c r="I47" s="8"/>
     </row>
-    <row r="48" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A48" s="6"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
+    <row r="48" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A48" s="9"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
       <c r="I48" s="8"/>
     </row>
-    <row r="49" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="6"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
+    <row r="49" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A49" s="9"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
       <c r="I49" s="8"/>
     </row>
-    <row r="50" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
+    <row r="50" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A50" s="9"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
       <c r="I50" s="8"/>
     </row>
-    <row r="51" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A51" s="12" t="s">
+    <row r="51" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="28" t="s">
+      <c r="B51" s="15"/>
+      <c r="C51" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
       <c r="I51" s="8"/>
     </row>
-    <row r="52" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A52" s="12" t="s">
+    <row r="52" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
       <c r="I52" s="8"/>
     </row>
-    <row r="53" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A53" s="6"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
+    <row r="53" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A53" s="9"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
       <c r="I53" s="8"/>
     </row>
-    <row r="54" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
       <c r="I54" s="8"/>
     </row>
-    <row r="55" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A55" s="6"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
+    <row r="55" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
       <c r="I55" s="8"/>
     </row>
-    <row r="56" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="26" t="s">
+      <c r="D56" s="15"/>
+      <c r="E56" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
       <c r="I56" s="8"/>
     </row>
-    <row r="57" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="26"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
       <c r="I57" s="8"/>
     </row>
-    <row r="58" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="26" t="s">
+      <c r="E58" s="15"/>
+      <c r="F58" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
       <c r="I58" s="8"/>
     </row>
-    <row r="59" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="6"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
+    <row r="59" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
       <c r="I59" s="8"/>
     </row>
-    <row r="60" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A60" s="6"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="26"/>
+    <row r="60" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
       <c r="I60" s="8"/>
     </row>
-    <row r="61" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A61" s="6"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
+    <row r="61" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A61" s="9"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
       <c r="I61" s="8"/>
     </row>
-    <row r="62" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A62" s="6"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
+    <row r="62" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A62" s="9"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
       <c r="I62" s="8"/>
     </row>
-    <row r="63" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A63" s="6"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
+    <row r="63" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A63" s="9"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
       <c r="I63" s="8"/>
     </row>
-    <row r="64" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A64" s="6"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="26"/>
-      <c r="G64" s="26"/>
-      <c r="H64" s="26"/>
+    <row r="64" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A64" s="9"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
       <c r="I64" s="8"/>
     </row>
-    <row r="65" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A65" s="6"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="26"/>
+    <row r="65" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A65" s="9"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
       <c r="I65" s="8"/>
     </row>
-    <row r="66" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A66" s="6"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="26"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="26"/>
-      <c r="I66" s="8"/>
-    </row>
-    <row r="67" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A67" s="13"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="15"/>
+    <row r="66" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="11"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Adjust the main page display and correct the content of SP.xlsx report.
</commit_message>
<xml_diff>
--- a/template/SP.xlsx
+++ b/template/SP.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E9C258-EA56-41C4-9943-27CA68982199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="SP" sheetId="1" r:id="rId1"/>
@@ -14,7 +13,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">SP!$A$1:$I$66</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">SP!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -155,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="[$-404]e&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
@@ -445,7 +444,7 @@
         <xdr:cNvPr id="2" name="圖片 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -495,7 +494,7 @@
         <xdr:cNvPr id="3" name="圖片 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -539,7 +538,7 @@
         <xdr:cNvPr id="4" name="圖片 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -583,7 +582,7 @@
         <xdr:cNvPr id="8" name="圖片 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -626,7 +625,7 @@
         <xdr:cNvPr id="9" name="圖片 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -663,14 +662,14 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>588066</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>56924</xdr:rowOff>
+      <xdr:rowOff>56925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="10" name="圖片 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -714,7 +713,7 @@
         <xdr:cNvPr id="11" name="圖片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -757,7 +756,7 @@
         <xdr:cNvPr id="12" name="圖片 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -787,9 +786,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -827,9 +826,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -864,7 +863,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -899,7 +898,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1072,11 +1071,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A34" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1124,7 @@
       </c>
       <c r="H4" s="21">
         <f ca="1">TODAY()</f>
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="I4" s="21"/>
     </row>
@@ -1467,7 +1466,7 @@
       <c r="H32" s="7"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>

</xml_diff>